<commit_message>
online harness time counting
</commit_message>
<xml_diff>
--- a/DB_connection/1821.xlsx
+++ b/DB_connection/1821.xlsx
@@ -626,8 +626,8 @@
   </sheetPr>
   <dimension ref="A1:Y256"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:Y255"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B242" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V257" activeCellId="0" sqref="V257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -771,6 +771,9 @@
       <c r="V3" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W3" s="0" t="n">
+        <v>200</v>
+      </c>
       <c r="X3" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -837,6 +840,9 @@
       <c r="V4" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W4" s="0" t="n">
+        <v>201</v>
+      </c>
       <c r="X4" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -903,6 +909,9 @@
       <c r="V5" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W5" s="0" t="n">
+        <v>202</v>
+      </c>
       <c r="X5" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -969,6 +978,9 @@
       <c r="V6" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W6" s="0" t="n">
+        <v>203</v>
+      </c>
       <c r="X6" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1035,6 +1047,9 @@
       <c r="V7" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W7" s="0" t="n">
+        <v>204</v>
+      </c>
       <c r="X7" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1101,6 +1116,9 @@
       <c r="V8" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W8" s="0" t="n">
+        <v>205</v>
+      </c>
       <c r="X8" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1167,6 +1185,9 @@
       <c r="V9" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W9" s="0" t="n">
+        <v>206</v>
+      </c>
       <c r="X9" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1233,6 +1254,9 @@
       <c r="V10" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W10" s="0" t="n">
+        <v>207</v>
+      </c>
       <c r="X10" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1299,6 +1323,9 @@
       <c r="V11" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W11" s="0" t="n">
+        <v>208</v>
+      </c>
       <c r="X11" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1365,6 +1392,9 @@
       <c r="V12" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W12" s="0" t="n">
+        <v>209</v>
+      </c>
       <c r="X12" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1431,6 +1461,9 @@
       <c r="V13" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W13" s="0" t="n">
+        <v>210</v>
+      </c>
       <c r="X13" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1497,6 +1530,9 @@
       <c r="V14" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W14" s="0" t="n">
+        <v>211</v>
+      </c>
       <c r="X14" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1563,6 +1599,9 @@
       <c r="V15" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W15" s="0" t="n">
+        <v>212</v>
+      </c>
       <c r="X15" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1629,6 +1668,9 @@
       <c r="V16" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W16" s="0" t="n">
+        <v>213</v>
+      </c>
       <c r="X16" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1695,6 +1737,9 @@
       <c r="V17" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W17" s="0" t="n">
+        <v>214</v>
+      </c>
       <c r="X17" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1761,6 +1806,9 @@
       <c r="V18" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W18" s="0" t="n">
+        <v>215</v>
+      </c>
       <c r="X18" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1818,6 +1866,9 @@
       <c r="T19" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W19" s="0" t="n">
+        <v>216</v>
+      </c>
       <c r="X19" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1875,6 +1926,9 @@
       <c r="T20" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W20" s="0" t="n">
+        <v>217</v>
+      </c>
       <c r="X20" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1932,6 +1986,9 @@
       <c r="T21" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W21" s="0" t="n">
+        <v>218</v>
+      </c>
       <c r="X21" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -1998,6 +2055,9 @@
       <c r="V22" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W22" s="0" t="n">
+        <v>219</v>
+      </c>
       <c r="X22" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2064,6 +2124,9 @@
       <c r="V23" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W23" s="0" t="n">
+        <v>220</v>
+      </c>
       <c r="X23" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2130,6 +2193,9 @@
       <c r="V24" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W24" s="0" t="n">
+        <v>221</v>
+      </c>
       <c r="X24" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2196,6 +2262,9 @@
       <c r="V25" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W25" s="0" t="n">
+        <v>222</v>
+      </c>
       <c r="X25" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2262,6 +2331,9 @@
       <c r="V26" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W26" s="0" t="n">
+        <v>223</v>
+      </c>
       <c r="X26" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2318,6 +2390,9 @@
       </c>
       <c r="T27" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="W27" s="0" t="n">
+        <v>224</v>
       </c>
       <c r="X27" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -2376,6 +2451,9 @@
       <c r="T28" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W28" s="0" t="n">
+        <v>225</v>
+      </c>
       <c r="X28" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2433,6 +2511,9 @@
       <c r="T29" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W29" s="0" t="n">
+        <v>226</v>
+      </c>
       <c r="X29" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2490,6 +2571,9 @@
       <c r="T30" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W30" s="0" t="n">
+        <v>227</v>
+      </c>
       <c r="X30" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2546,6 +2630,9 @@
       </c>
       <c r="T31" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="W31" s="0" t="n">
+        <v>228</v>
       </c>
       <c r="X31" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -2604,6 +2691,9 @@
       <c r="T32" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W32" s="0" t="n">
+        <v>229</v>
+      </c>
       <c r="X32" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2664,6 +2754,9 @@
       <c r="V33" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W33" s="0" t="n">
+        <v>230</v>
+      </c>
       <c r="X33" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2721,6 +2814,9 @@
       <c r="V34" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W34" s="0" t="n">
+        <v>231</v>
+      </c>
       <c r="X34" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2778,6 +2874,9 @@
       <c r="V35" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W35" s="0" t="n">
+        <v>232</v>
+      </c>
       <c r="X35" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2835,6 +2934,9 @@
       <c r="V36" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W36" s="0" t="n">
+        <v>233</v>
+      </c>
       <c r="X36" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2892,6 +2994,9 @@
       <c r="V37" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W37" s="0" t="n">
+        <v>234</v>
+      </c>
       <c r="X37" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -2949,6 +3054,9 @@
       <c r="V38" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W38" s="0" t="n">
+        <v>235</v>
+      </c>
       <c r="X38" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3006,6 +3114,9 @@
       <c r="V39" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W39" s="0" t="n">
+        <v>236</v>
+      </c>
       <c r="X39" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3063,6 +3174,9 @@
       <c r="V40" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W40" s="0" t="n">
+        <v>237</v>
+      </c>
       <c r="X40" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3120,6 +3234,9 @@
       <c r="V41" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W41" s="0" t="n">
+        <v>238</v>
+      </c>
       <c r="X41" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3177,6 +3294,9 @@
       <c r="V42" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W42" s="0" t="n">
+        <v>239</v>
+      </c>
       <c r="X42" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3234,6 +3354,9 @@
       <c r="V43" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W43" s="0" t="n">
+        <v>240</v>
+      </c>
       <c r="X43" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3291,6 +3414,9 @@
       <c r="V44" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W44" s="0" t="n">
+        <v>241</v>
+      </c>
       <c r="X44" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3348,6 +3474,9 @@
       <c r="V45" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W45" s="0" t="n">
+        <v>242</v>
+      </c>
       <c r="X45" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3408,6 +3537,9 @@
       <c r="V46" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W46" s="0" t="n">
+        <v>243</v>
+      </c>
       <c r="X46" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3468,6 +3600,9 @@
       <c r="V47" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W47" s="0" t="n">
+        <v>244</v>
+      </c>
       <c r="X47" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3528,6 +3663,9 @@
       <c r="V48" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W48" s="0" t="n">
+        <v>245</v>
+      </c>
       <c r="X48" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3585,6 +3723,9 @@
       <c r="V49" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W49" s="0" t="n">
+        <v>246</v>
+      </c>
       <c r="X49" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3642,6 +3783,9 @@
       <c r="V50" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W50" s="0" t="n">
+        <v>247</v>
+      </c>
       <c r="X50" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3699,6 +3843,9 @@
       <c r="V51" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W51" s="0" t="n">
+        <v>248</v>
+      </c>
       <c r="X51" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3756,6 +3903,9 @@
       <c r="V52" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W52" s="0" t="n">
+        <v>249</v>
+      </c>
       <c r="X52" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3813,6 +3963,9 @@
       <c r="V53" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W53" s="0" t="n">
+        <v>250</v>
+      </c>
       <c r="X53" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3870,6 +4023,9 @@
       <c r="V54" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W54" s="0" t="n">
+        <v>251</v>
+      </c>
       <c r="X54" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3927,6 +4083,9 @@
       <c r="V55" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W55" s="0" t="n">
+        <v>252</v>
+      </c>
       <c r="X55" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -3984,6 +4143,9 @@
       <c r="V56" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W56" s="0" t="n">
+        <v>253</v>
+      </c>
       <c r="X56" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4041,6 +4203,9 @@
       <c r="V57" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W57" s="0" t="n">
+        <v>254</v>
+      </c>
       <c r="X57" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4098,6 +4263,9 @@
       <c r="V58" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W58" s="0" t="n">
+        <v>255</v>
+      </c>
       <c r="X58" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4155,6 +4323,9 @@
       <c r="V59" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W59" s="0" t="n">
+        <v>256</v>
+      </c>
       <c r="X59" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4212,6 +4383,9 @@
       <c r="V60" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W60" s="0" t="n">
+        <v>257</v>
+      </c>
       <c r="X60" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4269,6 +4443,9 @@
       <c r="V61" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W61" s="0" t="n">
+        <v>258</v>
+      </c>
       <c r="X61" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4326,6 +4503,9 @@
       <c r="V62" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W62" s="0" t="n">
+        <v>259</v>
+      </c>
       <c r="X62" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4383,6 +4563,9 @@
       <c r="V63" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W63" s="0" t="n">
+        <v>260</v>
+      </c>
       <c r="X63" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4440,6 +4623,9 @@
       <c r="V64" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W64" s="0" t="n">
+        <v>261</v>
+      </c>
       <c r="X64" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4497,6 +4683,9 @@
       <c r="V65" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W65" s="0" t="n">
+        <v>262</v>
+      </c>
       <c r="X65" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4554,6 +4743,9 @@
       <c r="V66" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W66" s="0" t="n">
+        <v>263</v>
+      </c>
       <c r="X66" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4611,6 +4803,9 @@
       <c r="V67" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W67" s="0" t="n">
+        <v>264</v>
+      </c>
       <c r="X67" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4668,6 +4863,9 @@
       <c r="V68" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W68" s="0" t="n">
+        <v>265</v>
+      </c>
       <c r="X68" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4725,6 +4923,9 @@
       <c r="V69" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W69" s="0" t="n">
+        <v>266</v>
+      </c>
       <c r="X69" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4782,6 +4983,9 @@
       <c r="V70" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W70" s="0" t="n">
+        <v>267</v>
+      </c>
       <c r="X70" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4839,6 +5043,9 @@
       <c r="V71" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W71" s="0" t="n">
+        <v>268</v>
+      </c>
       <c r="X71" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4896,6 +5103,9 @@
       <c r="V72" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W72" s="0" t="n">
+        <v>269</v>
+      </c>
       <c r="X72" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -4953,6 +5163,9 @@
       <c r="V73" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W73" s="0" t="n">
+        <v>270</v>
+      </c>
       <c r="X73" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5010,6 +5223,9 @@
       <c r="V74" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W74" s="0" t="n">
+        <v>271</v>
+      </c>
       <c r="X74" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5067,6 +5283,9 @@
       <c r="V75" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W75" s="0" t="n">
+        <v>272</v>
+      </c>
       <c r="X75" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5124,6 +5343,9 @@
       <c r="V76" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W76" s="0" t="n">
+        <v>273</v>
+      </c>
       <c r="X76" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5181,6 +5403,9 @@
       <c r="V77" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W77" s="0" t="n">
+        <v>274</v>
+      </c>
       <c r="X77" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5238,6 +5463,9 @@
       <c r="V78" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W78" s="0" t="n">
+        <v>275</v>
+      </c>
       <c r="X78" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5295,6 +5523,9 @@
       <c r="V79" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W79" s="0" t="n">
+        <v>276</v>
+      </c>
       <c r="X79" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5352,6 +5583,9 @@
       <c r="V80" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W80" s="0" t="n">
+        <v>277</v>
+      </c>
       <c r="X80" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5409,6 +5643,9 @@
       <c r="V81" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W81" s="0" t="n">
+        <v>278</v>
+      </c>
       <c r="X81" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5466,6 +5703,9 @@
       <c r="V82" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W82" s="0" t="n">
+        <v>279</v>
+      </c>
       <c r="X82" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5523,6 +5763,9 @@
       <c r="V83" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W83" s="0" t="n">
+        <v>280</v>
+      </c>
       <c r="X83" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5580,6 +5823,9 @@
       <c r="V84" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W84" s="0" t="n">
+        <v>281</v>
+      </c>
       <c r="X84" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5637,6 +5883,9 @@
       <c r="V85" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W85" s="0" t="n">
+        <v>282</v>
+      </c>
       <c r="X85" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5694,6 +5943,9 @@
       <c r="V86" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W86" s="0" t="n">
+        <v>283</v>
+      </c>
       <c r="X86" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5751,6 +6003,9 @@
       <c r="V87" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W87" s="0" t="n">
+        <v>284</v>
+      </c>
       <c r="X87" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5808,6 +6063,9 @@
       <c r="V88" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W88" s="0" t="n">
+        <v>285</v>
+      </c>
       <c r="X88" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5865,6 +6123,9 @@
       <c r="V89" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W89" s="0" t="n">
+        <v>286</v>
+      </c>
       <c r="X89" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5922,6 +6183,9 @@
       <c r="V90" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W90" s="0" t="n">
+        <v>287</v>
+      </c>
       <c r="X90" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -5979,6 +6243,9 @@
       <c r="V91" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W91" s="0" t="n">
+        <v>288</v>
+      </c>
       <c r="X91" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6036,6 +6303,9 @@
       <c r="V92" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W92" s="0" t="n">
+        <v>289</v>
+      </c>
       <c r="X92" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6093,6 +6363,9 @@
       <c r="V93" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W93" s="0" t="n">
+        <v>290</v>
+      </c>
       <c r="X93" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6150,6 +6423,9 @@
       <c r="V94" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W94" s="0" t="n">
+        <v>291</v>
+      </c>
       <c r="X94" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6207,6 +6483,9 @@
       <c r="V95" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W95" s="0" t="n">
+        <v>292</v>
+      </c>
       <c r="X95" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6264,6 +6543,9 @@
       <c r="V96" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W96" s="0" t="n">
+        <v>293</v>
+      </c>
       <c r="X96" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6324,6 +6606,9 @@
       <c r="V97" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W97" s="0" t="n">
+        <v>294</v>
+      </c>
       <c r="X97" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6384,6 +6669,9 @@
       <c r="V98" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W98" s="0" t="n">
+        <v>295</v>
+      </c>
       <c r="X98" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6444,6 +6732,9 @@
       <c r="V99" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W99" s="0" t="n">
+        <v>296</v>
+      </c>
       <c r="X99" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6495,6 +6786,9 @@
       <c r="T100" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W100" s="0" t="n">
+        <v>297</v>
+      </c>
       <c r="X100" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6543,6 +6837,9 @@
       <c r="T101" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W101" s="0" t="n">
+        <v>298</v>
+      </c>
       <c r="X101" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6591,6 +6888,9 @@
       <c r="T102" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W102" s="0" t="n">
+        <v>299</v>
+      </c>
       <c r="X102" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6638,6 +6938,9 @@
       </c>
       <c r="T103" s="0" t="n">
         <v>16</v>
+      </c>
+      <c r="W103" s="0" t="n">
+        <v>300</v>
       </c>
       <c r="X103" s="0" t="n">
         <f aca="false">FALSE()</f>
@@ -6687,6 +6990,9 @@
       <c r="T104" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W104" s="0" t="n">
+        <v>301</v>
+      </c>
       <c r="X104" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6744,6 +7050,9 @@
       <c r="T105" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W105" s="0" t="n">
+        <v>302</v>
+      </c>
       <c r="X105" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6801,6 +7110,9 @@
       <c r="T106" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W106" s="0" t="n">
+        <v>303</v>
+      </c>
       <c r="X106" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6858,6 +7170,9 @@
       <c r="T107" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W107" s="0" t="n">
+        <v>304</v>
+      </c>
       <c r="X107" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6915,6 +7230,9 @@
       <c r="T108" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W108" s="0" t="n">
+        <v>305</v>
+      </c>
       <c r="X108" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -6972,6 +7290,9 @@
       <c r="T109" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W109" s="0" t="n">
+        <v>306</v>
+      </c>
       <c r="X109" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7029,6 +7350,9 @@
       <c r="T110" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W110" s="0" t="n">
+        <v>307</v>
+      </c>
       <c r="X110" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7095,6 +7419,9 @@
       <c r="V111" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W111" s="0" t="n">
+        <v>308</v>
+      </c>
       <c r="X111" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7152,6 +7479,9 @@
       <c r="T112" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W112" s="0" t="n">
+        <v>309</v>
+      </c>
       <c r="X112" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7209,6 +7539,9 @@
       <c r="T113" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W113" s="0" t="n">
+        <v>310</v>
+      </c>
       <c r="X113" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7266,6 +7599,9 @@
       <c r="T114" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W114" s="0" t="n">
+        <v>311</v>
+      </c>
       <c r="X114" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7326,6 +7662,9 @@
       <c r="V115" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W115" s="0" t="n">
+        <v>312</v>
+      </c>
       <c r="X115" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7383,6 +7722,9 @@
       <c r="V116" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W116" s="0" t="n">
+        <v>313</v>
+      </c>
       <c r="X116" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7440,6 +7782,9 @@
       <c r="V117" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W117" s="0" t="n">
+        <v>314</v>
+      </c>
       <c r="X117" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7497,6 +7842,9 @@
       <c r="V118" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W118" s="0" t="n">
+        <v>315</v>
+      </c>
       <c r="X118" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7554,6 +7902,9 @@
       <c r="V119" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="W119" s="0" t="n">
+        <v>316</v>
+      </c>
       <c r="X119" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7611,6 +7962,9 @@
       <c r="V120" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W120" s="0" t="n">
+        <v>317</v>
+      </c>
       <c r="X120" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7668,6 +8022,9 @@
       <c r="V121" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W121" s="0" t="n">
+        <v>318</v>
+      </c>
       <c r="X121" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7725,6 +8082,9 @@
       <c r="V122" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W122" s="0" t="n">
+        <v>319</v>
+      </c>
       <c r="X122" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7782,6 +8142,9 @@
       <c r="V123" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W123" s="0" t="n">
+        <v>320</v>
+      </c>
       <c r="X123" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7839,6 +8202,9 @@
       <c r="V124" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W124" s="0" t="n">
+        <v>321</v>
+      </c>
       <c r="X124" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7896,6 +8262,9 @@
       <c r="V125" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="W125" s="0" t="n">
+        <v>322</v>
+      </c>
       <c r="X125" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7944,6 +8313,9 @@
       <c r="T126" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W126" s="0" t="n">
+        <v>323</v>
+      </c>
       <c r="X126" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -7992,6 +8364,9 @@
       <c r="T127" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W127" s="0" t="n">
+        <v>324</v>
+      </c>
       <c r="X127" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8043,6 +8418,9 @@
       <c r="V128" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W128" s="0" t="n">
+        <v>325</v>
+      </c>
       <c r="X128" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8094,6 +8472,9 @@
       <c r="V129" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W129" s="0" t="n">
+        <v>326</v>
+      </c>
       <c r="X129" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8145,6 +8526,9 @@
       <c r="T130" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W130" s="0" t="n">
+        <v>327</v>
+      </c>
       <c r="X130" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8196,6 +8580,9 @@
       <c r="V131" s="0" t="s">
         <v>102</v>
       </c>
+      <c r="W131" s="0" t="n">
+        <v>328</v>
+      </c>
       <c r="X131" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8247,6 +8634,9 @@
       <c r="V132" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W132" s="0" t="n">
+        <v>329</v>
+      </c>
       <c r="X132" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8298,6 +8688,9 @@
       <c r="T133" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W133" s="0" t="n">
+        <v>330</v>
+      </c>
       <c r="X133" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8346,6 +8739,9 @@
       <c r="T134" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W134" s="0" t="n">
+        <v>331</v>
+      </c>
       <c r="X134" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8394,6 +8790,9 @@
       <c r="T135" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W135" s="0" t="n">
+        <v>332</v>
+      </c>
       <c r="X135" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8445,6 +8844,9 @@
       <c r="V136" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W136" s="0" t="n">
+        <v>333</v>
+      </c>
       <c r="X136" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8493,6 +8895,9 @@
       <c r="T137" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W137" s="0" t="n">
+        <v>334</v>
+      </c>
       <c r="X137" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8541,6 +8946,9 @@
       <c r="T138" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W138" s="0" t="n">
+        <v>335</v>
+      </c>
       <c r="X138" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8592,6 +9000,9 @@
       <c r="V139" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W139" s="0" t="n">
+        <v>336</v>
+      </c>
       <c r="X139" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8640,6 +9051,9 @@
       <c r="T140" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W140" s="0" t="n">
+        <v>337</v>
+      </c>
       <c r="X140" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8691,6 +9105,9 @@
       <c r="V141" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W141" s="0" t="n">
+        <v>338</v>
+      </c>
       <c r="X141" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8742,6 +9159,9 @@
       <c r="V142" s="0" t="s">
         <v>116</v>
       </c>
+      <c r="W142" s="0" t="n">
+        <v>339</v>
+      </c>
       <c r="X142" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8790,6 +9210,9 @@
       <c r="T143" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W143" s="0" t="n">
+        <v>340</v>
+      </c>
       <c r="X143" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8838,6 +9261,9 @@
       <c r="T144" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W144" s="0" t="n">
+        <v>341</v>
+      </c>
       <c r="X144" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8886,6 +9312,9 @@
       <c r="T145" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W145" s="0" t="n">
+        <v>342</v>
+      </c>
       <c r="X145" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -8952,6 +9381,9 @@
       <c r="V146" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="W146" s="0" t="n">
+        <v>343</v>
+      </c>
       <c r="X146" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9018,6 +9450,9 @@
       <c r="V147" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="W147" s="0" t="n">
+        <v>344</v>
+      </c>
       <c r="X147" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9084,6 +9519,9 @@
       <c r="V148" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="W148" s="0" t="n">
+        <v>345</v>
+      </c>
       <c r="X148" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9150,6 +9588,9 @@
       <c r="V149" s="0" t="s">
         <v>130</v>
       </c>
+      <c r="W149" s="0" t="n">
+        <v>346</v>
+      </c>
       <c r="X149" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9213,6 +9654,9 @@
       <c r="V150" s="0" t="s">
         <v>134</v>
       </c>
+      <c r="W150" s="0" t="n">
+        <v>347</v>
+      </c>
       <c r="X150" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9279,6 +9723,9 @@
       <c r="V151" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W151" s="0" t="n">
+        <v>348</v>
+      </c>
       <c r="X151" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9345,6 +9792,9 @@
       <c r="V152" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W152" s="0" t="n">
+        <v>349</v>
+      </c>
       <c r="X152" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9411,6 +9861,9 @@
       <c r="V153" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W153" s="0" t="n">
+        <v>350</v>
+      </c>
       <c r="X153" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9477,6 +9930,9 @@
       <c r="V154" s="0" t="s">
         <v>36</v>
       </c>
+      <c r="W154" s="0" t="n">
+        <v>351</v>
+      </c>
       <c r="X154" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9543,6 +9999,9 @@
       <c r="V155" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W155" s="0" t="n">
+        <v>352</v>
+      </c>
       <c r="X155" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9609,6 +10068,9 @@
       <c r="V156" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W156" s="0" t="n">
+        <v>353</v>
+      </c>
       <c r="X156" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9675,6 +10137,9 @@
       <c r="V157" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W157" s="0" t="n">
+        <v>354</v>
+      </c>
       <c r="X157" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9741,6 +10206,9 @@
       <c r="V158" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W158" s="0" t="n">
+        <v>355</v>
+      </c>
       <c r="X158" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9807,6 +10275,9 @@
       <c r="V159" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W159" s="0" t="n">
+        <v>356</v>
+      </c>
       <c r="X159" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9873,6 +10344,9 @@
       <c r="V160" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W160" s="0" t="n">
+        <v>357</v>
+      </c>
       <c r="X160" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -9939,6 +10413,9 @@
       <c r="V161" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W161" s="0" t="n">
+        <v>358</v>
+      </c>
       <c r="X161" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10005,6 +10482,9 @@
       <c r="V162" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W162" s="0" t="n">
+        <v>359</v>
+      </c>
       <c r="X162" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10071,6 +10551,9 @@
       <c r="V163" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W163" s="0" t="n">
+        <v>360</v>
+      </c>
       <c r="X163" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10137,6 +10620,9 @@
       <c r="V164" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W164" s="0" t="n">
+        <v>361</v>
+      </c>
       <c r="X164" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10203,6 +10689,9 @@
       <c r="V165" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W165" s="0" t="n">
+        <v>362</v>
+      </c>
       <c r="X165" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10269,6 +10758,9 @@
       <c r="V166" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W166" s="0" t="n">
+        <v>363</v>
+      </c>
       <c r="X166" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10335,6 +10827,9 @@
       <c r="V167" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W167" s="0" t="n">
+        <v>364</v>
+      </c>
       <c r="X167" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10401,6 +10896,9 @@
       <c r="V168" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W168" s="0" t="n">
+        <v>365</v>
+      </c>
       <c r="X168" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10467,6 +10965,9 @@
       <c r="V169" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W169" s="0" t="n">
+        <v>366</v>
+      </c>
       <c r="X169" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10533,6 +11034,9 @@
       <c r="V170" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W170" s="0" t="n">
+        <v>367</v>
+      </c>
       <c r="X170" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10599,6 +11103,9 @@
       <c r="V171" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W171" s="0" t="n">
+        <v>368</v>
+      </c>
       <c r="X171" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10665,6 +11172,9 @@
       <c r="V172" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W172" s="0" t="n">
+        <v>369</v>
+      </c>
       <c r="X172" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10731,6 +11241,9 @@
       <c r="V173" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W173" s="0" t="n">
+        <v>370</v>
+      </c>
       <c r="X173" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10797,6 +11310,9 @@
       <c r="V174" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W174" s="0" t="n">
+        <v>371</v>
+      </c>
       <c r="X174" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10863,6 +11379,9 @@
       <c r="V175" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W175" s="0" t="n">
+        <v>372</v>
+      </c>
       <c r="X175" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10929,6 +11448,9 @@
       <c r="V176" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W176" s="0" t="n">
+        <v>373</v>
+      </c>
       <c r="X176" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -10995,6 +11517,9 @@
       <c r="V177" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W177" s="0" t="n">
+        <v>374</v>
+      </c>
       <c r="X177" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11061,6 +11586,9 @@
       <c r="V178" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W178" s="0" t="n">
+        <v>375</v>
+      </c>
       <c r="X178" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11127,6 +11655,9 @@
       <c r="V179" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W179" s="0" t="n">
+        <v>376</v>
+      </c>
       <c r="X179" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11193,6 +11724,9 @@
       <c r="V180" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W180" s="0" t="n">
+        <v>377</v>
+      </c>
       <c r="X180" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11259,6 +11793,9 @@
       <c r="V181" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W181" s="0" t="n">
+        <v>378</v>
+      </c>
       <c r="X181" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11325,6 +11862,9 @@
       <c r="V182" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W182" s="0" t="n">
+        <v>379</v>
+      </c>
       <c r="X182" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11391,6 +11931,9 @@
       <c r="V183" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W183" s="0" t="n">
+        <v>380</v>
+      </c>
       <c r="X183" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11457,6 +12000,9 @@
       <c r="V184" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W184" s="0" t="n">
+        <v>381</v>
+      </c>
       <c r="X184" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11523,6 +12069,9 @@
       <c r="V185" s="0" t="s">
         <v>56</v>
       </c>
+      <c r="W185" s="0" t="n">
+        <v>382</v>
+      </c>
       <c r="X185" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11589,6 +12138,9 @@
       <c r="V186" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W186" s="0" t="n">
+        <v>383</v>
+      </c>
       <c r="X186" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11646,6 +12198,9 @@
       <c r="T187" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W187" s="0" t="n">
+        <v>384</v>
+      </c>
       <c r="X187" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11703,6 +12258,9 @@
       <c r="T188" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W188" s="0" t="n">
+        <v>385</v>
+      </c>
       <c r="X188" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11760,6 +12318,9 @@
       <c r="T189" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W189" s="0" t="n">
+        <v>386</v>
+      </c>
       <c r="X189" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11817,6 +12378,9 @@
       <c r="T190" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W190" s="0" t="n">
+        <v>387</v>
+      </c>
       <c r="X190" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11874,6 +12438,9 @@
       <c r="T191" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W191" s="0" t="n">
+        <v>388</v>
+      </c>
       <c r="X191" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -11940,6 +12507,9 @@
       <c r="V192" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W192" s="0" t="n">
+        <v>389</v>
+      </c>
       <c r="X192" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12006,6 +12576,9 @@
       <c r="V193" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W193" s="0" t="n">
+        <v>390</v>
+      </c>
       <c r="X193" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12072,6 +12645,9 @@
       <c r="V194" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W194" s="0" t="n">
+        <v>391</v>
+      </c>
       <c r="X194" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12138,6 +12714,9 @@
       <c r="V195" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W195" s="0" t="n">
+        <v>392</v>
+      </c>
       <c r="X195" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12204,6 +12783,9 @@
       <c r="V196" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W196" s="0" t="n">
+        <v>393</v>
+      </c>
       <c r="X196" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12270,6 +12852,9 @@
       <c r="V197" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W197" s="0" t="n">
+        <v>394</v>
+      </c>
       <c r="X197" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12336,6 +12921,9 @@
       <c r="V198" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W198" s="0" t="n">
+        <v>395</v>
+      </c>
       <c r="X198" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12402,6 +12990,9 @@
       <c r="V199" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W199" s="0" t="n">
+        <v>396</v>
+      </c>
       <c r="X199" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12468,6 +13059,9 @@
       <c r="V200" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W200" s="0" t="n">
+        <v>397</v>
+      </c>
       <c r="X200" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12534,6 +13128,9 @@
       <c r="V201" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W201" s="0" t="n">
+        <v>398</v>
+      </c>
       <c r="X201" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12600,6 +13197,9 @@
       <c r="V202" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W202" s="0" t="n">
+        <v>399</v>
+      </c>
       <c r="X202" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12666,6 +13266,9 @@
       <c r="V203" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W203" s="0" t="n">
+        <v>400</v>
+      </c>
       <c r="X203" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12732,6 +13335,9 @@
       <c r="V204" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W204" s="0" t="n">
+        <v>401</v>
+      </c>
       <c r="X204" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12798,6 +13404,9 @@
       <c r="V205" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W205" s="0" t="n">
+        <v>402</v>
+      </c>
       <c r="X205" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12864,6 +13473,9 @@
       <c r="V206" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W206" s="0" t="n">
+        <v>403</v>
+      </c>
       <c r="X206" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12930,6 +13542,9 @@
       <c r="V207" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W207" s="0" t="n">
+        <v>404</v>
+      </c>
       <c r="X207" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -12996,6 +13611,9 @@
       <c r="V208" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W208" s="0" t="n">
+        <v>405</v>
+      </c>
       <c r="X208" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13062,6 +13680,9 @@
       <c r="V209" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W209" s="0" t="n">
+        <v>406</v>
+      </c>
       <c r="X209" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13128,6 +13749,9 @@
       <c r="V210" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W210" s="0" t="n">
+        <v>407</v>
+      </c>
       <c r="X210" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13194,6 +13818,9 @@
       <c r="V211" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W211" s="0" t="n">
+        <v>408</v>
+      </c>
       <c r="X211" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13260,6 +13887,9 @@
       <c r="V212" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W212" s="0" t="n">
+        <v>409</v>
+      </c>
       <c r="X212" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13317,6 +13947,9 @@
       <c r="T213" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W213" s="0" t="n">
+        <v>410</v>
+      </c>
       <c r="X213" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13374,6 +14007,9 @@
       <c r="T214" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W214" s="0" t="n">
+        <v>411</v>
+      </c>
       <c r="X214" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13431,6 +14067,9 @@
       <c r="T215" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W215" s="0" t="n">
+        <v>412</v>
+      </c>
       <c r="X215" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13488,6 +14127,9 @@
       <c r="T216" s="0" t="n">
         <v>16</v>
       </c>
+      <c r="W216" s="0" t="n">
+        <v>413</v>
+      </c>
       <c r="X216" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13554,6 +14196,9 @@
       <c r="V217" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W217" s="0" t="n">
+        <v>414</v>
+      </c>
       <c r="X217" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13614,6 +14259,9 @@
       <c r="V218" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="W218" s="0" t="n">
+        <v>415</v>
+      </c>
       <c r="X218" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13674,6 +14322,9 @@
       <c r="V219" s="0" t="s">
         <v>127</v>
       </c>
+      <c r="W219" s="0" t="n">
+        <v>416</v>
+      </c>
       <c r="X219" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13734,6 +14385,9 @@
       <c r="V220" s="0" t="s">
         <v>39</v>
       </c>
+      <c r="W220" s="0" t="n">
+        <v>417</v>
+      </c>
       <c r="X220" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13791,6 +14445,9 @@
       <c r="V221" s="0" t="s">
         <v>68</v>
       </c>
+      <c r="W221" s="0" t="n">
+        <v>418</v>
+      </c>
       <c r="X221" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13848,6 +14505,9 @@
       <c r="V222" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W222" s="0" t="n">
+        <v>419</v>
+      </c>
       <c r="X222" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13905,6 +14565,9 @@
       <c r="V223" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W223" s="0" t="n">
+        <v>420</v>
+      </c>
       <c r="X223" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -13962,6 +14625,9 @@
       <c r="V224" s="0" t="s">
         <v>66</v>
       </c>
+      <c r="W224" s="0" t="n">
+        <v>421</v>
+      </c>
       <c r="X224" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14022,6 +14688,9 @@
       <c r="V225" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W225" s="0" t="n">
+        <v>422</v>
+      </c>
       <c r="X225" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14079,6 +14748,9 @@
       <c r="V226" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W226" s="0" t="n">
+        <v>423</v>
+      </c>
       <c r="X226" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14136,6 +14808,9 @@
       <c r="V227" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W227" s="0" t="n">
+        <v>424</v>
+      </c>
       <c r="X227" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14193,6 +14868,9 @@
       <c r="V228" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W228" s="0" t="n">
+        <v>425</v>
+      </c>
       <c r="X228" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14250,6 +14928,9 @@
       <c r="V229" s="0" t="s">
         <v>44</v>
       </c>
+      <c r="W229" s="0" t="n">
+        <v>426</v>
+      </c>
       <c r="X229" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14310,6 +14991,9 @@
       <c r="V230" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W230" s="0" t="n">
+        <v>427</v>
+      </c>
       <c r="X230" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14370,6 +15054,9 @@
       <c r="V231" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W231" s="0" t="n">
+        <v>428</v>
+      </c>
       <c r="X231" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14430,6 +15117,9 @@
       <c r="V232" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W232" s="0" t="n">
+        <v>429</v>
+      </c>
       <c r="X232" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14490,6 +15180,9 @@
       <c r="V233" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W233" s="0" t="n">
+        <v>430</v>
+      </c>
       <c r="X233" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14550,6 +15243,9 @@
       <c r="V234" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W234" s="0" t="n">
+        <v>431</v>
+      </c>
       <c r="X234" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14610,6 +15306,9 @@
       <c r="V235" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W235" s="0" t="n">
+        <v>432</v>
+      </c>
       <c r="X235" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14670,6 +15369,9 @@
       <c r="V236" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W236" s="0" t="n">
+        <v>433</v>
+      </c>
       <c r="X236" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14730,6 +15432,9 @@
       <c r="V237" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W237" s="0" t="n">
+        <v>434</v>
+      </c>
       <c r="X237" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14787,6 +15492,9 @@
       <c r="V238" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W238" s="0" t="n">
+        <v>435</v>
+      </c>
       <c r="X238" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14844,6 +15552,9 @@
       <c r="V239" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W239" s="0" t="n">
+        <v>436</v>
+      </c>
       <c r="X239" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14901,6 +15612,9 @@
       <c r="V240" s="0" t="s">
         <v>50</v>
       </c>
+      <c r="W240" s="0" t="n">
+        <v>437</v>
+      </c>
       <c r="X240" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -14958,6 +15672,9 @@
       <c r="V241" s="0" t="s">
         <v>52</v>
       </c>
+      <c r="W241" s="0" t="n">
+        <v>438</v>
+      </c>
       <c r="X241" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15018,6 +15735,9 @@
       <c r="V242" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W242" s="0" t="n">
+        <v>439</v>
+      </c>
       <c r="X242" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15078,6 +15798,9 @@
       <c r="V243" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W243" s="0" t="n">
+        <v>440</v>
+      </c>
       <c r="X243" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15138,6 +15861,9 @@
       <c r="V244" s="0" t="s">
         <v>57</v>
       </c>
+      <c r="W244" s="0" t="n">
+        <v>441</v>
+      </c>
       <c r="X244" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15189,6 +15915,9 @@
       <c r="T245" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W245" s="0" t="n">
+        <v>442</v>
+      </c>
       <c r="X245" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15240,6 +15969,9 @@
       <c r="T246" s="0" t="n">
         <v>5.2</v>
       </c>
+      <c r="W246" s="0" t="n">
+        <v>443</v>
+      </c>
       <c r="X246" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15306,6 +16038,9 @@
       <c r="V247" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="W247" s="0" t="n">
+        <v>444</v>
+      </c>
       <c r="X247" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15372,6 +16107,9 @@
       <c r="V248" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W248" s="0" t="n">
+        <v>445</v>
+      </c>
       <c r="X248" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15438,6 +16176,9 @@
       <c r="V249" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W249" s="0" t="n">
+        <v>446</v>
+      </c>
       <c r="X249" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15504,6 +16245,9 @@
       <c r="V250" s="0" t="s">
         <v>112</v>
       </c>
+      <c r="W250" s="0" t="n">
+        <v>447</v>
+      </c>
       <c r="X250" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15570,6 +16314,9 @@
       <c r="V251" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W251" s="0" t="n">
+        <v>448</v>
+      </c>
       <c r="X251" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15636,6 +16383,9 @@
       <c r="V252" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W252" s="0" t="n">
+        <v>449</v>
+      </c>
       <c r="X252" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15696,6 +16446,9 @@
       <c r="V253" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W253" s="0" t="n">
+        <v>450</v>
+      </c>
       <c r="X253" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15756,6 +16509,9 @@
       <c r="V254" s="0" t="s">
         <v>107</v>
       </c>
+      <c r="W254" s="0" t="n">
+        <v>451</v>
+      </c>
       <c r="X254" s="0" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
@@ -15803,6 +16559,9 @@
       </c>
       <c r="T255" s="0" t="n">
         <v>5.2</v>
+      </c>
+      <c r="W255" s="0" t="n">
+        <v>452</v>
       </c>
       <c r="X255" s="0" t="n">
         <f aca="false">FALSE()</f>

</xml_diff>